<commit_message>
upload all actors added
</commit_message>
<xml_diff>
--- a/public/files/excel-template/parent-template.xlsx
+++ b/public/files/excel-template/parent-template.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OJOago ELEVATE\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hdtl\edulite\public\files\excel-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E7DF8D3-ECA7-4673-B20F-3E85AB21F56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC522405-074C-4B02-9C91-F444052E96EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{76F13B92-220A-4085-B44B-8CF4A5FB621A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="NOTE" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>firstname</t>
   </si>
@@ -44,23 +45,56 @@
     <t>othername</t>
   </si>
   <si>
-    <t>gam</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
     <t>address</t>
   </si>
   <si>
-    <t>wards</t>
+    <t>religion</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>gsm</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GENDER </t>
+  </si>
+  <si>
+    <t>RELIGION</t>
+  </si>
+  <si>
+    <t>the number coresponding number represent each gender</t>
+  </si>
+  <si>
+    <t>the corresponding number represent each religion</t>
+  </si>
+  <si>
+    <t>MALE</t>
+  </si>
+  <si>
+    <t>MUSLIM</t>
+  </si>
+  <si>
+    <t>FEMALE</t>
+  </si>
+  <si>
+    <t>CHRISTIAN</t>
+  </si>
+  <si>
+    <t>OTHER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,16 +102,68 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="48"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -85,12 +171,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,39 +542,169 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{231FCEAD-7AEC-4E6A-9902-E8A9E5227095}">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55CB80A3-FCDB-44C2-888E-79EFA8DC4A95}">
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="6">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="use 1 for Male, 2 for Female and 3 for other" sqref="I1:I1048576" xr:uid="{D2FCC902-DCDD-4C70-A970-B054F7E2963B}">
+      <formula1>1</formula1>
+      <formula2>3</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="use 1 for Muslim, 2 for Christain and 3 for Other" sqref="H1:H1048576" xr:uid="{23C3E29C-9B20-4D71-B4DA-8568B0186D4F}">
+      <formula1>1</formula1>
+      <formula2>3</formula2>
+    </dataValidation>
+    <dataValidation type="textLength" operator="equal" showInputMessage="1" showErrorMessage="1" error="10 digits, omit the first 0" promptTitle="phone number" sqref="D1:D1048576" xr:uid="{14D0E4FB-FBD0-4433-92BA-AA8976A557EE}">
+      <formula1>10</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="lessThan" showInputMessage="1" showErrorMessage="1" error="maximum of 30 character" sqref="B1:B1048576" xr:uid="{901F6D0F-8E63-4994-95BA-2CEECA45D2D8}">
+      <formula1>30</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="maximum of 30 character" sqref="A1:A1048576" xr:uid="{565B5BC9-404A-43F3-836B-4BEE4DD29ECD}">
+      <formula1>31</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="address is compulsary and not more than 255 characters" sqref="G1" xr:uid="{17DBBBF0-1FC2-4349-91A1-B7BDC286D217}">
+      <formula1>256</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C25C0A-0DBB-4D95-9B16-F4B5D1662B2D}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="D2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" ht="61.5" x14ac:dyDescent="0.9">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="61.5" x14ac:dyDescent="0.9">
+      <c r="A4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="7">
+        <v>2</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="61.5" x14ac:dyDescent="0.9">
+      <c r="A5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="7">
+        <v>3</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D8:E8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>